<commit_message>
updated data dicitonary with unique constraints and removed movies_info table
</commit_message>
<xml_diff>
--- a/lab1/data_dictionary.xlsx
+++ b/lab1/data_dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="1" r:id="rId1"/>
@@ -21,15 +21,14 @@
     <sheet name="Movies" sheetId="8" r:id="rId7"/>
     <sheet name="Movies_Genres" sheetId="9" r:id="rId8"/>
     <sheet name="Movies_Keywords" sheetId="10" r:id="rId9"/>
-    <sheet name="Movie_Info" sheetId="11" r:id="rId10"/>
-    <sheet name="Series" sheetId="12" r:id="rId11"/>
+    <sheet name="Series" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="58">
   <si>
     <t>Column names</t>
   </si>
@@ -202,10 +201,7 @@
     <t>not null constraint</t>
   </si>
   <si>
-    <t>idmovies</t>
-  </si>
-  <si>
-    <t>idmovies_info</t>
+    <t>not null and unique constraint</t>
   </si>
 </sst>
 </file>
@@ -629,7 +625,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -641,7 +637,7 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>12</v>
@@ -28654,116 +28650,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28812,7 +28702,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -28823,7 +28713,7 @@
         <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>54</v>
@@ -28895,7 +28785,7 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28948,7 +28838,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -28959,7 +28849,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>11</v>
@@ -29055,7 +28945,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -29066,7 +28956,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>17</v>
@@ -29095,8 +28985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29145,7 +29035,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -29156,7 +29046,7 @@
         <v>26</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>28</v>
@@ -29225,7 +29115,7 @@
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29274,7 +29164,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -29285,7 +29175,7 @@
         <v>27</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>29</v>
@@ -29371,7 +29261,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29420,7 +29310,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>38</v>
       </c>
@@ -29432,7 +29322,7 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>39</v>
@@ -57424,7 +57314,7 @@
   <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -57476,7 +57366,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -57487,7 +57377,7 @@
         <v>30</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>42</v>
@@ -57565,7 +57455,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -57618,7 +57508,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -57629,7 +57519,7 @@
         <v>46</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>47</v>
@@ -57702,7 +57592,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -57769,7 +57659,7 @@
         <v>50</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>51</v>
@@ -57778,7 +57668,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Updated DDL with data type revisions and alters
</commit_message>
<xml_diff>
--- a/lab1/data_dictionary.xlsx
+++ b/lab1/data_dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="59">
   <si>
     <t>Column names</t>
   </si>
@@ -162,9 +162,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>language</t>
-  </si>
-  <si>
     <t>id_movies_genres</t>
   </si>
   <si>
@@ -202,6 +199,12 @@
   </si>
   <si>
     <t>not null and unique constraint</t>
+  </si>
+  <si>
+    <t>char(1)</t>
+  </si>
+  <si>
+    <t>char(3)</t>
   </si>
 </sst>
 </file>
@@ -566,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -637,7 +640,7 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>12</v>
@@ -772,7 +775,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -28652,8 +28655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28713,10 +28716,10 @@
         <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>33</v>
@@ -28741,10 +28744,10 @@
         <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>24</v>
@@ -28752,13 +28755,13 @@
     </row>
     <row r="5" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
@@ -28849,7 +28852,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>11</v>
@@ -28869,7 +28872,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>9</v>
@@ -28956,7 +28959,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>17</v>
@@ -29046,7 +29049,7 @@
         <v>26</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>28</v>
@@ -29066,7 +29069,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>30</v>
@@ -29175,7 +29178,7 @@
         <v>27</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>29</v>
@@ -29322,7 +29325,7 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>39</v>
@@ -29360,7 +29363,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="8" t="s">
@@ -57313,8 +57316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -57377,7 +57380,7 @@
         <v>30</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>42</v>
@@ -57423,8 +57426,12 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="G6" s="3" t="s">
         <v>43</v>
       </c>
@@ -57432,17 +57439,13 @@
     <row r="7" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="G7" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="G8" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
   </sheetData>
@@ -57452,10 +57455,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -57510,22 +57513,22 @@
     </row>
     <row r="2" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
@@ -57539,7 +57542,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>30</v>
@@ -57556,30 +57559,10 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -57650,22 +57633,22 @@
     </row>
     <row r="2" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
@@ -57679,7 +57662,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>30</v>
@@ -57696,7 +57679,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>38</v>
@@ -57710,7 +57693,7 @@
         <v>33</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>